<commit_message>
Major rewrite of the program.
The input file format has changed, as has the command line arguments. The program now requires the anytree module.
</commit_message>
<xml_diff>
--- a/demo-input.xlsx
+++ b/demo-input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wallace/Documents/Lab-All/Lab-Projects/GIT/asct-b-generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA178BE4-9DC2-D148-B7F4-95FAF4EF43B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11104D84-5BB9-FE4C-9777-9051B5C0487E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50280" yWindow="5740" windowWidth="35580" windowHeight="22260" xr2:uid="{155688E7-F6B7-EE44-84E0-60F83BBFF981}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
   <si>
     <t>TYPE</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>REFERENCES (DOI)</t>
+  </si>
+  <si>
+    <t>CELLS</t>
   </si>
 </sst>
 </file>
@@ -589,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90DD31CA-2F20-0644-8236-F5678D8C767A}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -602,16 +605,17 @@
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
@@ -627,29 +631,32 @@
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -663,7 +670,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -677,7 +684,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -691,7 +698,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -704,11 +711,11 @@
       <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -721,11 +728,11 @@
       <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -738,11 +745,11 @@
       <c r="D7" t="s">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -755,11 +762,11 @@
       <c r="D8" t="s">
         <v>2</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -769,23 +776,23 @@
       <c r="D9" t="s">
         <v>3</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>8</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>17</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>27</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>28</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -795,20 +802,20 @@
       <c r="D10" t="s">
         <v>3</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>12</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>31</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>32</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -818,23 +825,23 @@
       <c r="D11" t="s">
         <v>3</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>11</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>14</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>26</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>28</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -842,7 +849,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -850,7 +857,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -858,7 +865,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -866,7 +873,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
added "note" and "ABBR" (abbreviation) fields for each feature
</commit_message>
<xml_diff>
--- a/demo-input.xlsx
+++ b/demo-input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wallace/Documents/Lab-All/Lab-Projects/GIT/asct-b-generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11104D84-5BB9-FE4C-9777-9051B5C0487E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236C6884-C8AE-3843-8F2D-D87233E24831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50280" yWindow="5740" windowWidth="35580" windowHeight="22260" xr2:uid="{155688E7-F6B7-EE44-84E0-60F83BBFF981}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="25140" xr2:uid="{155688E7-F6B7-EE44-84E0-60F83BBFF981}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="69">
   <si>
     <t>TYPE</t>
   </si>
@@ -235,6 +235,12 @@
   </si>
   <si>
     <t>CELLS</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>ABBR</t>
   </si>
 </sst>
 </file>
@@ -592,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90DD31CA-2F20-0644-8236-F5678D8C767A}">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -603,19 +609,20 @@
     <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
@@ -626,79 +633,85 @@
         <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>50</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>51</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>52</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -708,14 +721,14 @@
       <c r="C5" t="s">
         <v>53</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>2</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -725,14 +738,14 @@
       <c r="C6" t="s">
         <v>54</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>2</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -742,14 +755,14 @@
       <c r="C7" t="s">
         <v>55</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>2</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -759,181 +772,181 @@
       <c r="C8" t="s">
         <v>56</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>2</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>3</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>8</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>17</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>27</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>28</v>
       </c>
-      <c r="M9" t="s">
+      <c r="O9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>3</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" t="s">
         <v>12</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
         <v>31</v>
       </c>
-      <c r="J10" t="s">
+      <c r="L10" t="s">
         <v>32</v>
       </c>
-      <c r="M10" t="s">
+      <c r="O10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>3</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I11" t="s">
         <v>11</v>
       </c>
-      <c r="H11" t="s">
+      <c r="J11" t="s">
         <v>14</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>26</v>
       </c>
-      <c r="K11" t="s">
+      <c r="M11" t="s">
         <v>28</v>
       </c>
-      <c r="M11" t="s">
+      <c r="O11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="D14" t="s">
+      <c r="F14" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="D15" t="s">
+      <c r="F15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>25</v>
       </c>
-      <c r="D17" t="s">
+      <c r="F17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="D18" t="s">
+      <c r="F18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>27</v>
       </c>
-      <c r="D19" t="s">
+      <c r="F19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>32</v>
       </c>
-      <c r="D20" t="s">
+      <c r="F20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>28</v>
       </c>
-      <c r="D21" t="s">
+      <c r="F21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>29</v>
       </c>
-      <c r="D22" t="s">
+      <c r="F22" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>30</v>
       </c>
-      <c r="D23" t="s">
+      <c r="F23" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated demo for input header.
</commit_message>
<xml_diff>
--- a/demo-input.xlsx
+++ b/demo-input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wallace/Documents/Lab-All/Lab-Projects/GIT/asct-b-generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236C6884-C8AE-3843-8F2D-D87233E24831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6860E64-3BD1-D944-8715-5FDF4E7333B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="25140" xr2:uid="{155688E7-F6B7-EE44-84E0-60F83BBFF981}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="80">
   <si>
     <t>TYPE</t>
   </si>
@@ -241,19 +241,84 @@
   </si>
   <si>
     <t>ABBR</t>
+  </si>
+  <si>
+    <r>
+      <t>Anatomical Structures, Cell Types and Biomarkers Table for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;insert organ name&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Author Name(s):</t>
+  </si>
+  <si>
+    <t>Author ORCID(s):</t>
+  </si>
+  <si>
+    <t>Reviewer(s):</t>
+  </si>
+  <si>
+    <t>Reviewer ORCID(s):</t>
+  </si>
+  <si>
+    <t>General Publication(s):</t>
+  </si>
+  <si>
+    <t>Data DOI:</t>
+  </si>
+  <si>
+    <t>Will be added after table is finalized and published</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>Version Number:</t>
+  </si>
+  <si>
+    <t>v</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -276,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -284,6 +349,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90DD31CA-2F20-0644-8236-F5678D8C767A}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,331 +690,395 @@
     <col min="15" max="15" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="5">
+        <v>44652</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O11" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J9" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9" t="s">
-        <v>27</v>
-      </c>
-      <c r="M9" t="s">
-        <v>28</v>
-      </c>
-      <c r="O9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" t="s">
-        <v>3</v>
-      </c>
-      <c r="I10" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" t="s">
-        <v>31</v>
-      </c>
-      <c r="L10" t="s">
-        <v>32</v>
-      </c>
-      <c r="O10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" t="s">
-        <v>26</v>
-      </c>
-      <c r="M11" t="s">
-        <v>28</v>
-      </c>
-      <c r="O11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
       </c>
       <c r="F14" t="s">
-        <v>44</v>
+        <v>2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
       </c>
       <c r="F15" t="s">
-        <v>45</v>
+        <v>2</v>
+      </c>
+      <c r="H15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" t="s">
+        <v>17</v>
+      </c>
+      <c r="L19" t="s">
+        <v>27</v>
+      </c>
+      <c r="M19" t="s">
+        <v>28</v>
+      </c>
+      <c r="O19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" t="s">
+        <v>31</v>
+      </c>
+      <c r="L20" t="s">
+        <v>32</v>
+      </c>
+      <c r="O20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" t="s">
+        <v>3</v>
+      </c>
+      <c r="I21" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" t="s">
         <v>14</v>
       </c>
-      <c r="F16" t="s">
+      <c r="K21" t="s">
+        <v>26</v>
+      </c>
+      <c r="M21" t="s">
+        <v>28</v>
+      </c>
+      <c r="O21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>26</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F28" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>27</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F29" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>32</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F30" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F31" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>29</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F32" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>30</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F33" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>